<commit_message>
Final Resume4 and created Assignment5
</commit_message>
<xml_diff>
--- a/Week4. Correct requirements and life cycle/Resume.xlsx
+++ b/Week4. Correct requirements and life cycle/Resume.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>Фамилия</t>
   </si>
@@ -49,13 +49,52 @@
     <t>Руданов</t>
   </si>
   <si>
-    <t>Примечание</t>
-  </si>
-  <si>
-    <t>рецензист</t>
-  </si>
-  <si>
-    <t>отвечающий</t>
+    <t>Задание</t>
+  </si>
+  <si>
+    <t>Степень выполнения</t>
+  </si>
+  <si>
+    <t>Назначение системы, рецензирование документации второй подгруппы</t>
+  </si>
+  <si>
+    <t>Пользовательские требования, работа компоненты тестирования (как будет происходить проверка задач)</t>
+  </si>
+  <si>
+    <t>Проектирование сущностей и связей БД, черновик календарногоплана проекта, выбор жизненного цикла</t>
+  </si>
+  <si>
+    <t>Рецензирование документации второй подгруппы</t>
+  </si>
+  <si>
+    <t>Выбор жизненного цикла</t>
+  </si>
+  <si>
+    <t>Написание глоссария</t>
+  </si>
+  <si>
+    <t>Составление новой версии требований</t>
+  </si>
+  <si>
+    <t>Цели системы, подготовка к ответу на семинаре</t>
+  </si>
+  <si>
+    <t>Выбор языка программирования и среды разработки с обоснованием, подготовка к ответу на семинаре</t>
+  </si>
+  <si>
+    <t>Сорокин</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Черновик календарного плана проекта</t>
+  </si>
+  <si>
+    <t>Выполнено</t>
+  </si>
+  <si>
+    <t>Не выполнено</t>
   </si>
 </sst>
 </file>
@@ -71,7 +110,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -92,7 +131,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -109,11 +154,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -418,20 +467,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="101.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -439,79 +489,150 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
       <c r="C2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
       <c r="C5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="B8">
         <v>8</v>
       </c>
-      <c r="B8">
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
+      <c r="B9">
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>